<commit_message>
Fixed Great Britain x United Kingdom mismatch in the freedom index data
</commit_message>
<xml_diff>
--- a/Tools and meta-analysis theory/Freedom index/master_data.xlsx
+++ b/Tools and meta-analysis theory/Freedom index/master_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Tools and meta-analysis theory\Freedom index\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7610F64-CBC5-4A6D-A532-BCB4FCF51CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AEAD36-684E-4547-8A63-714250005497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="50">
   <si>
     <t>data_avgyear</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>Slovakia</t>
-  </si>
-  <si>
-    <t>Great Britain</t>
   </si>
   <si>
     <t>Brazil</t>
@@ -717,7 +714,7 @@
   <dimension ref="A1:B1755"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11347,7 +11344,7 @@
         <v>1984</v>
       </c>
       <c r="B1328" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1329" spans="1:2" x14ac:dyDescent="0.25">
@@ -11355,7 +11352,7 @@
         <v>1984</v>
       </c>
       <c r="B1329" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1330" spans="1:2" x14ac:dyDescent="0.25">
@@ -11363,7 +11360,7 @@
         <v>1984</v>
       </c>
       <c r="B1330" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1331" spans="1:2" x14ac:dyDescent="0.25">
@@ -11371,7 +11368,7 @@
         <v>1984</v>
       </c>
       <c r="B1331" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1332" spans="1:2" x14ac:dyDescent="0.25">
@@ -11379,7 +11376,7 @@
         <v>1984</v>
       </c>
       <c r="B1332" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1333" spans="1:2" x14ac:dyDescent="0.25">
@@ -11387,7 +11384,7 @@
         <v>1984</v>
       </c>
       <c r="B1333" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1334" spans="1:2" x14ac:dyDescent="0.25">
@@ -11395,7 +11392,7 @@
         <v>1984</v>
       </c>
       <c r="B1334" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1335" spans="1:2" x14ac:dyDescent="0.25">
@@ -11403,7 +11400,7 @@
         <v>1984</v>
       </c>
       <c r="B1335" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1336" spans="1:2" x14ac:dyDescent="0.25">
@@ -11411,7 +11408,7 @@
         <v>1984</v>
       </c>
       <c r="B1336" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1337" spans="1:2" x14ac:dyDescent="0.25">
@@ -11419,7 +11416,7 @@
         <v>1984</v>
       </c>
       <c r="B1337" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1338" spans="1:2" x14ac:dyDescent="0.25">
@@ -11427,7 +11424,7 @@
         <v>1984</v>
       </c>
       <c r="B1338" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1339" spans="1:2" x14ac:dyDescent="0.25">
@@ -11435,7 +11432,7 @@
         <v>1984</v>
       </c>
       <c r="B1339" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1340" spans="1:2" x14ac:dyDescent="0.25">
@@ -11443,7 +11440,7 @@
         <v>1984</v>
       </c>
       <c r="B1340" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1341" spans="1:2" x14ac:dyDescent="0.25">
@@ -11451,7 +11448,7 @@
         <v>1984</v>
       </c>
       <c r="B1341" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1342" spans="1:2" x14ac:dyDescent="0.25">
@@ -11459,7 +11456,7 @@
         <v>1984</v>
       </c>
       <c r="B1342" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1343" spans="1:2" x14ac:dyDescent="0.25">
@@ -11467,7 +11464,7 @@
         <v>1980</v>
       </c>
       <c r="B1343" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1344" spans="1:2" x14ac:dyDescent="0.25">
@@ -11475,7 +11472,7 @@
         <v>1980</v>
       </c>
       <c r="B1344" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1345" spans="1:2" x14ac:dyDescent="0.25">
@@ -11483,7 +11480,7 @@
         <v>1980</v>
       </c>
       <c r="B1345" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1346" spans="1:2" x14ac:dyDescent="0.25">
@@ -11491,7 +11488,7 @@
         <v>1980</v>
       </c>
       <c r="B1346" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1347" spans="1:2" x14ac:dyDescent="0.25">
@@ -11499,7 +11496,7 @@
         <v>1980</v>
       </c>
       <c r="B1347" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1348" spans="1:2" x14ac:dyDescent="0.25">
@@ -11507,7 +11504,7 @@
         <v>1980</v>
       </c>
       <c r="B1348" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1349" spans="1:2" x14ac:dyDescent="0.25">
@@ -11515,7 +11512,7 @@
         <v>1980</v>
       </c>
       <c r="B1349" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1350" spans="1:2" x14ac:dyDescent="0.25">
@@ -12427,7 +12424,7 @@
         <v>1986</v>
       </c>
       <c r="B1463" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1464" spans="1:2" x14ac:dyDescent="0.25">
@@ -12435,7 +12432,7 @@
         <v>1991</v>
       </c>
       <c r="B1464" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1465" spans="1:2" x14ac:dyDescent="0.25">
@@ -12443,7 +12440,7 @@
         <v>1997</v>
       </c>
       <c r="B1465" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1466" spans="1:2" x14ac:dyDescent="0.25">
@@ -12451,7 +12448,7 @@
         <v>1998</v>
       </c>
       <c r="B1466" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1467" spans="1:2" x14ac:dyDescent="0.25">
@@ -12459,7 +12456,7 @@
         <v>2000</v>
       </c>
       <c r="B1467" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1468" spans="1:2" x14ac:dyDescent="0.25">
@@ -12467,7 +12464,7 @@
         <v>2002</v>
       </c>
       <c r="B1468" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1469" spans="1:2" x14ac:dyDescent="0.25">
@@ -12507,7 +12504,7 @@
         <v>1997</v>
       </c>
       <c r="B1473" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1474" spans="1:2" x14ac:dyDescent="0.25">
@@ -12515,7 +12512,7 @@
         <v>1998</v>
       </c>
       <c r="B1474" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1475" spans="1:2" x14ac:dyDescent="0.25">
@@ -12523,7 +12520,7 @@
         <v>2000</v>
       </c>
       <c r="B1475" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1476" spans="1:2" x14ac:dyDescent="0.25">
@@ -12531,7 +12528,7 @@
         <v>2002</v>
       </c>
       <c r="B1476" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="1477" spans="1:2" x14ac:dyDescent="0.25">
@@ -13171,7 +13168,7 @@
         <v>1986</v>
       </c>
       <c r="B1556" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1557" spans="1:2" x14ac:dyDescent="0.25">
@@ -13179,7 +13176,7 @@
         <v>1986</v>
       </c>
       <c r="B1557" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1558" spans="1:2" x14ac:dyDescent="0.25">
@@ -13187,7 +13184,7 @@
         <v>1986</v>
       </c>
       <c r="B1558" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1559" spans="1:2" x14ac:dyDescent="0.25">
@@ -13195,7 +13192,7 @@
         <v>1986</v>
       </c>
       <c r="B1559" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1560" spans="1:2" x14ac:dyDescent="0.25">
@@ -13203,7 +13200,7 @@
         <v>1986</v>
       </c>
       <c r="B1560" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1561" spans="1:2" x14ac:dyDescent="0.25">
@@ -13227,7 +13224,7 @@
         <v>1985</v>
       </c>
       <c r="B1563" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1564" spans="1:2" x14ac:dyDescent="0.25">
@@ -13235,7 +13232,7 @@
         <v>1985</v>
       </c>
       <c r="B1564" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1565" spans="1:2" x14ac:dyDescent="0.25">
@@ -13243,7 +13240,7 @@
         <v>1985</v>
       </c>
       <c r="B1565" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1566" spans="1:2" x14ac:dyDescent="0.25">
@@ -13251,7 +13248,7 @@
         <v>1985</v>
       </c>
       <c r="B1566" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1567" spans="1:2" x14ac:dyDescent="0.25">
@@ -13259,7 +13256,7 @@
         <v>1985</v>
       </c>
       <c r="B1567" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1568" spans="1:2" x14ac:dyDescent="0.25">
@@ -13267,7 +13264,7 @@
         <v>1985</v>
       </c>
       <c r="B1568" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1569" spans="1:2" x14ac:dyDescent="0.25">
@@ -13275,7 +13272,7 @@
         <v>1985</v>
       </c>
       <c r="B1569" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1570" spans="1:2" x14ac:dyDescent="0.25">
@@ -13283,7 +13280,7 @@
         <v>1985</v>
       </c>
       <c r="B1570" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1571" spans="1:2" x14ac:dyDescent="0.25">
@@ -13291,7 +13288,7 @@
         <v>1985</v>
       </c>
       <c r="B1571" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1572" spans="1:2" x14ac:dyDescent="0.25">
@@ -13891,7 +13888,7 @@
         <v>1971</v>
       </c>
       <c r="B1646" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1647" spans="1:2" x14ac:dyDescent="0.25">
@@ -13899,7 +13896,7 @@
         <v>1971</v>
       </c>
       <c r="B1647" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1648" spans="1:2" x14ac:dyDescent="0.25">
@@ -13907,7 +13904,7 @@
         <v>1971</v>
       </c>
       <c r="B1648" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1649" spans="1:2" x14ac:dyDescent="0.25">
@@ -13915,7 +13912,7 @@
         <v>1971</v>
       </c>
       <c r="B1649" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1650" spans="1:2" x14ac:dyDescent="0.25">
@@ -13923,7 +13920,7 @@
         <v>1971</v>
       </c>
       <c r="B1650" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1651" spans="1:2" x14ac:dyDescent="0.25">
@@ -13931,7 +13928,7 @@
         <v>1971</v>
       </c>
       <c r="B1651" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1652" spans="1:2" x14ac:dyDescent="0.25">
@@ -13939,7 +13936,7 @@
         <v>1973</v>
       </c>
       <c r="B1652" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1653" spans="1:2" x14ac:dyDescent="0.25">
@@ -13947,7 +13944,7 @@
         <v>1973</v>
       </c>
       <c r="B1653" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1654" spans="1:2" x14ac:dyDescent="0.25">
@@ -13955,7 +13952,7 @@
         <v>1973</v>
       </c>
       <c r="B1654" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1655" spans="1:2" x14ac:dyDescent="0.25">
@@ -13963,7 +13960,7 @@
         <v>1973</v>
       </c>
       <c r="B1655" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1656" spans="1:2" x14ac:dyDescent="0.25">
@@ -13971,7 +13968,7 @@
         <v>1973</v>
       </c>
       <c r="B1656" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1657" spans="1:2" x14ac:dyDescent="0.25">
@@ -13979,7 +13976,7 @@
         <v>1973</v>
       </c>
       <c r="B1657" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="1658" spans="1:2" x14ac:dyDescent="0.25">
@@ -14251,7 +14248,7 @@
         <v>1989</v>
       </c>
       <c r="B1691" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1692" spans="1:2" x14ac:dyDescent="0.25">
@@ -14259,7 +14256,7 @@
         <v>1989</v>
       </c>
       <c r="B1692" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="1693" spans="1:2" x14ac:dyDescent="0.25">
@@ -14291,7 +14288,7 @@
         <v>1972</v>
       </c>
       <c r="B1696" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1697" spans="1:2" x14ac:dyDescent="0.25">
@@ -14299,7 +14296,7 @@
         <v>1972</v>
       </c>
       <c r="B1697" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1698" spans="1:2" x14ac:dyDescent="0.25">
@@ -14307,7 +14304,7 @@
         <v>1972</v>
       </c>
       <c r="B1698" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1699" spans="1:2" x14ac:dyDescent="0.25">
@@ -14315,7 +14312,7 @@
         <v>1972</v>
       </c>
       <c r="B1699" s="9" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1700" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>